<commit_message>
remove camel from popup
</commit_message>
<xml_diff>
--- a/config/languageFile.xlsx
+++ b/config/languageFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenn\Nextcloud\Artikel Cognitive Affective Maps Tools\CAM tools\CAMtools_CAMEL\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\CAM TOOLS\TOOLS\Data Collection Tool\DataCollection\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270CF9F5-82C0-4D0D-AF82-A66E216DA304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E794EA7-C268-48DA-984D-DEF1B879D415}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1057,12 +1057,6 @@
     <t>Ihre CAM-Daten wurden an den Sever gesendet. Wir danken Ihnen für Ihre Teilnahme! Sie werden zum Ende oder zum letzten Teil der Studie weitergeleitet.</t>
   </si>
   <si>
-    <t>You would have send the CAM data successfully to a sever. To save permanently your data please use our administrative panel or host the C.A.M.E.L. software on your own server.</t>
-  </si>
-  <si>
-    <t>Sie hätten die CAM-Daten erfolgreich an einen Server gesendet. Um Ihre Daten dauerhaft zu speichern, verwenden Sie bitte unser Administrationspanel oder hosten Sie die C.A.M.E.L. Software auf Ihrem eigenen Server.</t>
-  </si>
-  <si>
     <t>popSave_01notSavedData</t>
   </si>
   <si>
@@ -1246,9 +1240,6 @@
     <t>Los datos de su Cognitive-Affective Map se han mandado al servidor. Gracias por participación! Usted será llevado al final de la sesión o a su última parte.</t>
   </si>
   <si>
-    <t>Usted habría mandado los datos de su CAM al servidor con éxito. Para guardar sus datos de forma permanente, por favor use nuestro panel de administración o aloje C.A.M.E.L. en su propio servidor.</t>
-  </si>
-  <si>
     <t>En cambio, por favor traze varios conceptos conectados.</t>
   </si>
   <si>
@@ -1486,9 +1477,6 @@
     <t>Vos données de la CAM ont été envoyées au serveur. Nous vous remercions de votre participation ! Vous allez être redirigé vers la fin ou la dernière partie de l'étude.</t>
   </si>
   <si>
-    <t>Vous avez envoyé avec succès vos données CAM à un serveur. Pour sauvegarder vos données de manière permanente, veuillez utiliser notre panneau d'administration ou héberger le logiciel C.A.M.E.L. sur votre propre serveur.</t>
-  </si>
-  <si>
     <t>Veuillez plutôt dessiner plusieurs concepts cohérents.</t>
   </si>
   <si>
@@ -1901,6 +1889,18 @@
   </si>
   <si>
     <t>alert loading (to force fullscreen and avoid errors)</t>
+  </si>
+  <si>
+    <t>You would have send the CAM data successfully to a sever. To save permanently your data please use our administrative panel or host the software on your own server.</t>
+  </si>
+  <si>
+    <t>Sie hätten die CAM-Daten erfolgreich an einen Server gesendet. Um Ihre Daten dauerhaft zu speichern, verwenden Sie bitte unser Administrationspanel oder hosten Sie die Software auf Ihrem eigenen Server.</t>
+  </si>
+  <si>
+    <t>Vous avez envoyé avec succès vos données CAM à un serveur. Pour sauvegarder vos données de manière permanente, veuillez utiliser notre panneau d'administration ou héberger le logiciel sur votre propre serveur.</t>
+  </si>
+  <si>
+    <t>Usted habría mandado los datos de su CAM al servidor con éxito. Para guardar sus datos de forma permanente, por favor use nuestro panel de administración o aloje en su propio servidor.</t>
   </si>
 </sst>
 </file>
@@ -2310,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2343,7 +2343,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>56</v>
@@ -2366,13 +2366,13 @@
         <v>202</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>201</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -2391,13 +2391,13 @@
         <v>109</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>110</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2416,13 +2416,13 @@
         <v>111</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>112</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -2441,13 +2441,13 @@
         <v>114</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>113</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -2466,13 +2466,13 @@
         <v>115</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>116</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2491,13 +2491,13 @@
         <v>117</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>119</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2516,13 +2516,13 @@
         <v>118</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>120</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2541,13 +2541,13 @@
         <v>121</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>123</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2566,13 +2566,13 @@
         <v>122</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>124</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2591,13 +2591,13 @@
         <v>125</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>126</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -2616,13 +2616,13 @@
         <v>192</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>160</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -2635,19 +2635,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>127</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>129</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -2666,13 +2666,13 @@
         <v>128</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>199</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
@@ -2691,13 +2691,13 @@
         <v>130</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>131</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -2716,13 +2716,13 @@
         <v>132</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>133</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -2741,13 +2741,13 @@
         <v>134</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>154</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2766,13 +2766,13 @@
         <v>135</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>153</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -2791,13 +2791,13 @@
         <v>140</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>152</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -2816,13 +2816,13 @@
         <v>137</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>136</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -2841,13 +2841,13 @@
         <v>138</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>139</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -2866,13 +2866,13 @@
         <v>157</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>141</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -2891,13 +2891,13 @@
         <v>142</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>143</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -2916,13 +2916,13 @@
         <v>144</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>145</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -2941,13 +2941,13 @@
         <v>146</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>147</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -2966,13 +2966,13 @@
         <v>148</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>149</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -2991,13 +2991,13 @@
         <v>150</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>151</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -3016,13 +3016,13 @@
         <v>155</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>156</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -3041,13 +3041,13 @@
         <v>158</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>161</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -3066,13 +3066,13 @@
         <v>207</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>208</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -3091,13 +3091,13 @@
         <v>159</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>165</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -3116,13 +3116,13 @@
         <v>163</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>162</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -3141,13 +3141,13 @@
         <v>164</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>166</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3166,13 +3166,13 @@
         <v>167</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>168</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3191,13 +3191,13 @@
         <v>223</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>228</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3216,13 +3216,13 @@
         <v>224</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>227</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3241,13 +3241,13 @@
         <v>225</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>226</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3266,13 +3266,13 @@
         <v>169</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>170</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3297,7 +3297,7 @@
         <v>172</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3316,13 +3316,13 @@
         <v>173</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>174</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -3341,13 +3341,13 @@
         <v>66</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>175</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -3366,13 +3366,13 @@
         <v>176</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>177</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
@@ -3391,13 +3391,13 @@
         <v>178</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>179</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
@@ -3416,13 +3416,13 @@
         <v>180</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>181</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -3441,13 +3441,13 @@
         <v>182</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>183</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -3466,13 +3466,13 @@
         <v>184</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>185</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
@@ -3491,13 +3491,13 @@
         <v>186</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>187</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -3516,13 +3516,13 @@
         <v>188</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>189</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
@@ -3535,19 +3535,19 @@
         <v>84</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>541</v>
       </c>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
@@ -3566,13 +3566,13 @@
         <v>210</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>211</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
@@ -3591,13 +3591,13 @@
         <v>190</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>191</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -3616,13 +3616,13 @@
         <v>230</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>231</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
@@ -3635,10 +3635,10 @@
         <v>92</v>
       </c>
       <c r="C53" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="D53" s="9" t="s">
         <v>526</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>530</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>200</v>
@@ -3647,7 +3647,7 @@
         <v>194</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
@@ -3660,19 +3660,19 @@
         <v>92</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>193</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
@@ -3691,13 +3691,13 @@
         <v>195</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>196</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
@@ -3716,13 +3716,13 @@
         <v>163</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>162</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -3741,13 +3741,13 @@
         <v>198</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>197</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
@@ -3766,13 +3766,13 @@
         <v>217</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>218</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
@@ -3791,13 +3791,13 @@
         <v>247</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -3816,29 +3816,29 @@
         <v>246</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
     <row r="61" spans="1:9" ht="60">
       <c r="A61" s="2" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>232</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
@@ -3848,16 +3848,16 @@
     </row>
     <row r="62" spans="1:9" ht="30">
       <c r="A62" s="2" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>232</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -3879,13 +3879,13 @@
         <v>239</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
@@ -3904,13 +3904,13 @@
         <v>240</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
@@ -3932,10 +3932,10 @@
         <v>238</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
@@ -3954,13 +3954,13 @@
         <v>257</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
@@ -3979,13 +3979,13 @@
         <v>258</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
@@ -4004,13 +4004,13 @@
         <v>257</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
@@ -4029,13 +4029,13 @@
         <v>259</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
@@ -4054,13 +4054,13 @@
         <v>260</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
@@ -4079,498 +4079,498 @@
         <v>263</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="1:9" ht="150">
+    <row r="72" spans="1:9" ht="135">
       <c r="A72" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>232</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>264</v>
+        <v>542</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>265</v>
+        <v>543</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>407</v>
+        <v>544</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>327</v>
+        <v>545</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
     </row>
     <row r="73" spans="1:9" ht="60">
       <c r="A73" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
     </row>
     <row r="74" spans="1:9" ht="60">
       <c r="A74" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
     </row>
     <row r="75" spans="1:9" ht="30">
       <c r="A75" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="D75" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
     <row r="76" spans="1:9" ht="30">
       <c r="A76" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
     <row r="77" spans="1:9" ht="30">
       <c r="A77" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
     </row>
     <row r="78" spans="1:9" ht="30">
       <c r="A78" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
     <row r="79" spans="1:9" ht="45">
       <c r="A79" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
     </row>
     <row r="80" spans="1:9" ht="60">
       <c r="A80" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
     <row r="81" spans="1:9" ht="45">
       <c r="A81" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
     </row>
     <row r="82" spans="1:9" ht="45">
       <c r="A82" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>293</v>
-      </c>
       <c r="D82" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
     </row>
     <row r="83" spans="1:9" ht="45">
       <c r="A83" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
     </row>
     <row r="84" spans="1:9" ht="45">
       <c r="A84" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
     </row>
     <row r="85" spans="1:9" ht="45">
       <c r="A85" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="C85" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
     </row>
     <row r="86" spans="1:9" ht="150">
       <c r="A86" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
     </row>
     <row r="87" spans="1:9" ht="75">
       <c r="A87" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="C87" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
     </row>
     <row r="88" spans="1:9" ht="90">
       <c r="A88" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="D88" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="D89" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="D90" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>73</v>
@@ -4579,54 +4579,54 @@
         <v>109</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>110</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
     </row>
     <row r="92" spans="1:9" ht="30">
       <c r="A92" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>355</v>
-      </c>
       <c r="G92" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
     </row>
     <row r="93" spans="1:9" ht="45">
       <c r="A93" s="7" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>

</xml_diff>